<commit_message>
version 2 with plottings
</commit_message>
<xml_diff>
--- a/data/helper_data.xlsx
+++ b/data/helper_data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sean/Seans Mac Pro/KUMED/의예과/학생연구/Nerve-Morphology-2.0/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{967011D3-BAA1-3040-8909-364BF99FD62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EABE282-5043-CB41-8123-AC6689546CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7580" yWindow="2700" windowWidth="27900" windowHeight="16940" xr2:uid="{DF547B5D-F6B7-1846-8137-FFFBF5C7594C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{DF547B5D-F6B7-1846-8137-FFFBF5C7594C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="28">
   <si>
     <t>23-21R</t>
   </si>
@@ -107,13 +107,27 @@
   </si>
   <si>
     <t>sp_y</t>
+  </si>
+  <si>
+    <t>23-49R</t>
+  </si>
+  <si>
+    <t>23-49L</t>
+  </si>
+  <si>
+    <t>24-10L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>24-10R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -128,6 +142,19 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Malgun Gothic"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,8 +179,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -470,15 +503,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB16A65-966F-0F4D-A686-8143472BB790}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:19">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -521,8 +554,20 @@
       <c r="O1" t="s">
         <v>13</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -557,7 +602,7 @@
         <v>16.584292099999999</v>
       </c>
       <c r="L2">
-        <v>25.071428600000001</v>
+        <v>9.2147988990108995</v>
       </c>
       <c r="M2">
         <v>20.357142899999999</v>
@@ -568,8 +613,20 @@
       <c r="O2">
         <v>11.575287599999999</v>
       </c>
+      <c r="P2">
+        <v>25</v>
+      </c>
+      <c r="Q2">
+        <v>25</v>
+      </c>
+      <c r="R2">
+        <v>30</v>
+      </c>
+      <c r="S2">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -603,8 +660,32 @@
       <c r="K3" t="s">
         <v>16</v>
       </c>
+      <c r="L3">
+        <v>3.9874535999999998</v>
+      </c>
+      <c r="M3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3">
+        <v>0.99873000000000001</v>
+      </c>
+      <c r="O3" s="2">
+        <v>3.8453309999999998</v>
+      </c>
+      <c r="P3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3">
+        <v>4.2319321258972815</v>
+      </c>
+      <c r="S3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -638,8 +719,32 @@
       <c r="K4" t="s">
         <v>16</v>
       </c>
+      <c r="L4">
+        <v>8.0656789095063477</v>
+      </c>
+      <c r="M4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>10.54368</v>
+      </c>
+      <c r="P4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4">
+        <v>25.823288344357017</v>
+      </c>
+      <c r="S4" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -673,8 +778,32 @@
       <c r="K5" t="s">
         <v>16</v>
       </c>
+      <c r="L5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" s="2">
+        <v>2.1579578000000001</v>
+      </c>
+      <c r="P5">
+        <v>0.66227141950951773</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>16</v>
+      </c>
+      <c r="R5" t="s">
+        <v>16</v>
+      </c>
+      <c r="S5">
+        <v>2.5006000483279482</v>
+      </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -708,8 +837,33 @@
       <c r="K6" t="s">
         <v>16</v>
       </c>
+      <c r="L6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O6">
+        <f>O4*0.4</f>
+        <v>4.2174719999999999</v>
+      </c>
+      <c r="P6">
+        <v>0.85547379999999995</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>16</v>
+      </c>
+      <c r="R6" t="s">
+        <v>16</v>
+      </c>
+      <c r="S6">
+        <v>10.522248837991638</v>
+      </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -743,8 +897,32 @@
       <c r="K7" t="s">
         <v>16</v>
       </c>
+      <c r="L7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" t="s">
+        <v>16</v>
+      </c>
+      <c r="O7" t="s">
+        <v>16</v>
+      </c>
+      <c r="P7">
+        <v>-0.44145839178950902</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>16</v>
+      </c>
+      <c r="R7" t="s">
+        <v>16</v>
+      </c>
+      <c r="S7">
+        <v>3.2872743003149614</v>
+      </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -778,8 +956,32 @@
       <c r="K8" t="s">
         <v>16</v>
       </c>
+      <c r="L8" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" t="s">
+        <v>16</v>
+      </c>
+      <c r="O8" t="s">
+        <v>16</v>
+      </c>
+      <c r="P8">
+        <v>1.1447638913992391</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>16</v>
+      </c>
+      <c r="R8" t="s">
+        <v>16</v>
+      </c>
+      <c r="S8">
+        <v>7.7038360800672789</v>
+      </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -801,8 +1003,8 @@
       <c r="G9" t="s">
         <v>16</v>
       </c>
-      <c r="H9" t="s">
-        <v>16</v>
+      <c r="H9">
+        <v>1.9663820000000001</v>
       </c>
       <c r="I9" t="s">
         <v>16</v>
@@ -813,8 +1015,29 @@
       <c r="K9" t="s">
         <v>16</v>
       </c>
+      <c r="L9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" t="s">
+        <v>16</v>
+      </c>
+      <c r="N9" t="s">
+        <v>16</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>16</v>
+      </c>
+      <c r="R9">
+        <v>1.3178299277337395</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -836,8 +1059,8 @@
       <c r="G10" t="s">
         <v>16</v>
       </c>
-      <c r="H10" t="s">
-        <v>16</v>
+      <c r="H10">
+        <v>1.19733636</v>
       </c>
       <c r="I10" t="s">
         <v>16</v>
@@ -847,6 +1070,28 @@
       </c>
       <c r="K10" t="s">
         <v>16</v>
+      </c>
+      <c r="L10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N10" t="s">
+        <v>16</v>
+      </c>
+      <c r="O10">
+        <f>O4*0.3</f>
+        <v>3.1631040000000001</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>16</v>
+      </c>
+      <c r="R10">
+        <v>12.724681595629225</v>
+      </c>
+      <c r="S10">
+        <v>-1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>